<commit_message>
Add visualisation config to simple chart survey for coverage
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/programs-charting-simple-valid.xlsx
+++ b/packages/central-server/__tests__/importers/programs-charting-simple-valid.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>programName</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>Size</t>
+  </si>
+  <si>
+    <t>{"min": 0, "max": 300, "normalRange": {"min": 90, "max": 120}}</t>
+  </si>
+  <si>
+    <t>{"yAxis":{"graphRange":{"min":40,"max":240},"interval":10}}</t>
   </si>
   <si>
     <t>testchartcode3</t>
@@ -159,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -169,6 +175,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,8 +201,8 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1563,7 +1574,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1606,19 +1617,25 @@
       <c r="D4" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="K4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat(desktopCharting): SAV-773: Add complex chart graph importer validation (#8145)
* Prevent complex chart surveys to have visualisation config

* Create unit test coverage

* Create xlsx file for unit case

* Add visualisation config to simple chart survey for coverage

* Reverse check order and improve unit test check

* refactor(tests): SAV-773: Split programs importer test file (#8151)

* Refactor into smaller files

* Remove unneded table truncates per file and declare them inline on hook, also ditch doing that on afterAll hook
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/programs-charting-simple-valid.xlsx
+++ b/packages/central-server/__tests__/importers/programs-charting-simple-valid.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>programName</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>Size</t>
+  </si>
+  <si>
+    <t>{"min": 0, "max": 300, "normalRange": {"min": 90, "max": 120}}</t>
+  </si>
+  <si>
+    <t>{"yAxis":{"graphRange":{"min":40,"max":240},"interval":10}}</t>
   </si>
   <si>
     <t>testchartcode3</t>
@@ -159,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -169,6 +175,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,8 +201,8 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1563,7 +1574,7 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1606,19 +1617,25 @@
       <c r="D4" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="K4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>

</xml_diff>